<commit_message>
Fixing indicators bugs (overage learners) and including age in school-cycle's labels
</commit_message>
<xml_diff>
--- a/input_tool/edu_analysistools_loa_AFG.xlsx
+++ b/input_tool/edu_analysistools_loa_AFG.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acted-my.sharepoint.com/personal/martina_vit_impact-initiatives_org/Documents/MSNAEdu/EduAnalysisTool/input_tool/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="284" documentId="13_ncr:1_{C3CB7579-362D-4DB3-A6E6-0B702A8819F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D00EC2E3-B57F-4682-AE89-2B8089E1B6B2}"/>
+  <xr:revisionPtr revIDLastSave="286" documentId="13_ncr:1_{C3CB7579-362D-4DB3-A6E6-0B702A8819F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{177256AF-91BD-4805-8C69-A9F4D4CC8F82}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" xr2:uid="{172E695D-8722-4AF3-920F-94814F3A8B09}"/>
   </bookViews>
@@ -209,7 +209,7 @@
     <t>edu_school_cycle_d, admin2</t>
   </si>
   <si>
-    <t>overage</t>
+    <t>overaged</t>
   </si>
 </sst>
 </file>
@@ -1071,10 +1071,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFE1FF5D-95CC-49D0-8C54-8D9CF98199B7}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:L133"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="F76" sqref="F76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -1123,7 +1124,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1161,7 +1162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1199,7 +1200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -1237,7 +1238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -1275,7 +1276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1313,7 +1314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -1351,7 +1352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -1389,7 +1390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -1427,7 +1428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1465,7 +1466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -1503,7 +1504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1541,7 +1542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -1579,7 +1580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -1617,7 +1618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -1655,7 +1656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -1693,7 +1694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -1731,7 +1732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -1769,7 +1770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -1807,7 +1808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -1845,7 +1846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -1883,7 +1884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -1921,7 +1922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -1959,7 +1960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -1997,7 +1998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -2035,7 +2036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A26" t="s">
         <v>7</v>
       </c>
@@ -2073,7 +2074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A27" t="s">
         <v>20</v>
       </c>
@@ -2111,7 +2112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A28" t="s">
         <v>22</v>
       </c>
@@ -2149,7 +2150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A29" t="s">
         <v>24</v>
       </c>
@@ -2187,7 +2188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A30" t="s">
         <v>7</v>
       </c>
@@ -2225,7 +2226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A31" t="s">
         <v>20</v>
       </c>
@@ -2263,7 +2264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A32" t="s">
         <v>22</v>
       </c>
@@ -2301,7 +2302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A33" t="s">
         <v>24</v>
       </c>
@@ -2339,7 +2340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A34" t="s">
         <v>7</v>
       </c>
@@ -2377,7 +2378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A35" t="s">
         <v>20</v>
       </c>
@@ -2415,7 +2416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -2453,7 +2454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="37" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A37" t="s">
         <v>24</v>
       </c>
@@ -2491,7 +2492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A38" t="s">
         <v>7</v>
       </c>
@@ -2529,7 +2530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="39" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A39" t="s">
         <v>20</v>
       </c>
@@ -2567,7 +2568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="40" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A40" t="s">
         <v>22</v>
       </c>
@@ -2605,7 +2606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="41" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A41" t="s">
         <v>24</v>
       </c>
@@ -2643,7 +2644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A42" t="s">
         <v>30</v>
       </c>
@@ -2681,7 +2682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="43" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A43" t="s">
         <v>26</v>
       </c>
@@ -2719,7 +2720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="44" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A44" t="s">
         <v>30</v>
       </c>
@@ -2757,7 +2758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="45" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A45" t="s">
         <v>26</v>
       </c>
@@ -2795,7 +2796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="46" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A46" t="s">
         <v>30</v>
       </c>
@@ -2833,7 +2834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="47" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A47" t="s">
         <v>26</v>
       </c>
@@ -2871,7 +2872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="48" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A48" t="s">
         <v>30</v>
       </c>
@@ -2909,7 +2910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="49" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A49" t="s">
         <v>26</v>
       </c>
@@ -2947,7 +2948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="50" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A50" t="s">
         <v>30</v>
       </c>
@@ -2985,7 +2986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="51" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A51" t="s">
         <v>26</v>
       </c>
@@ -3023,7 +3024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="52" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A52" t="s">
         <v>30</v>
       </c>
@@ -3061,7 +3062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="53" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A53" t="s">
         <v>26</v>
       </c>
@@ -3099,7 +3100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="54" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A54" t="s">
         <v>26</v>
       </c>
@@ -3137,7 +3138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="55" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A55" t="s">
         <v>30</v>
       </c>
@@ -3175,7 +3176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="56" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A56" t="s">
         <v>26</v>
       </c>
@@ -3213,7 +3214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="57" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A57" t="s">
         <v>30</v>
       </c>
@@ -3251,7 +3252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="58" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A58" t="s">
         <v>30</v>
       </c>
@@ -3289,7 +3290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="59" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A59" t="s">
         <v>26</v>
       </c>
@@ -3327,7 +3328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="60" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A60" t="s">
         <v>30</v>
       </c>
@@ -3365,7 +3366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="61" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A61" t="s">
         <v>26</v>
       </c>
@@ -3403,7 +3404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="62" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A62" t="s">
         <v>10</v>
       </c>
@@ -3441,7 +3442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="63" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A63" t="s">
         <v>10</v>
       </c>
@@ -3479,7 +3480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="64" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.75">
       <c r="A64" s="2" t="s">
         <v>10</v>
       </c>
@@ -3517,7 +3518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="65" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.75">
       <c r="A65" s="2" t="s">
         <v>10</v>
       </c>
@@ -3555,7 +3556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="66" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A66" t="s">
         <v>10</v>
       </c>
@@ -3593,7 +3594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="67" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A67" t="s">
         <v>10</v>
       </c>
@@ -3631,7 +3632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="68" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A68" t="s">
         <v>10</v>
       </c>
@@ -3669,7 +3670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:12" ht="15" x14ac:dyDescent="0.75">
+    <row r="69" spans="1:12" ht="15" hidden="1" x14ac:dyDescent="0.75">
       <c r="A69" t="s">
         <v>11</v>
       </c>
@@ -3707,7 +3708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:12" ht="15" x14ac:dyDescent="0.75">
+    <row r="70" spans="1:12" ht="15" hidden="1" x14ac:dyDescent="0.75">
       <c r="A70" t="s">
         <v>11</v>
       </c>
@@ -3745,7 +3746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:12" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.75">
+    <row r="71" spans="1:12" s="2" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.75">
       <c r="A71" s="2" t="s">
         <v>11</v>
       </c>
@@ -3783,7 +3784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:12" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.75">
+    <row r="72" spans="1:12" s="2" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.75">
       <c r="A72" s="2" t="s">
         <v>11</v>
       </c>
@@ -3821,7 +3822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:12" ht="15" x14ac:dyDescent="0.75">
+    <row r="73" spans="1:12" ht="15" hidden="1" x14ac:dyDescent="0.75">
       <c r="A73" t="s">
         <v>11</v>
       </c>
@@ -3859,7 +3860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:12" ht="15" x14ac:dyDescent="0.75">
+    <row r="74" spans="1:12" ht="15" hidden="1" x14ac:dyDescent="0.75">
       <c r="A74" t="s">
         <v>11</v>
       </c>
@@ -3897,7 +3898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:12" ht="15" x14ac:dyDescent="0.75">
+    <row r="75" spans="1:12" ht="15" hidden="1" x14ac:dyDescent="0.75">
       <c r="A75" t="s">
         <v>11</v>
       </c>
@@ -4733,7 +4734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="97" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A97" t="s">
         <v>36</v>
       </c>
@@ -4771,7 +4772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="98" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A98" t="s">
         <v>36</v>
       </c>
@@ -4809,7 +4810,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="99" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A99" t="s">
         <v>36</v>
       </c>
@@ -4847,7 +4848,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="100" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A100" t="s">
         <v>36</v>
       </c>
@@ -4885,7 +4886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="101" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A101" t="s">
         <v>36</v>
       </c>
@@ -4923,7 +4924,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="102" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A102" t="s">
         <v>36</v>
       </c>
@@ -4961,7 +4962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="103" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A103" t="s">
         <v>37</v>
       </c>
@@ -4999,7 +5000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="104" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A104" t="s">
         <v>37</v>
       </c>
@@ -5037,7 +5038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="105" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A105" t="s">
         <v>37</v>
       </c>
@@ -5075,7 +5076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="106" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A106" t="s">
         <v>37</v>
       </c>
@@ -5113,7 +5114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="107" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A107" t="s">
         <v>37</v>
       </c>
@@ -5151,7 +5152,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="108" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A108" t="s">
         <v>37</v>
       </c>
@@ -5189,7 +5190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="109" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.75">
       <c r="A109" s="2" t="s">
         <v>7</v>
       </c>
@@ -5227,7 +5228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="110" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.75">
       <c r="A110" s="2" t="s">
         <v>7</v>
       </c>
@@ -5265,7 +5266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="111" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A111" t="s">
         <v>7</v>
       </c>
@@ -5303,7 +5304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="112" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A112" t="s">
         <v>7</v>
       </c>
@@ -5341,7 +5342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="113" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A113" t="s">
         <v>7</v>
       </c>
@@ -5379,7 +5380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="114" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A114" t="s">
         <v>18</v>
       </c>
@@ -5417,7 +5418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="115" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A115" t="s">
         <v>18</v>
       </c>
@@ -5455,7 +5456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="116" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A116" t="s">
         <v>18</v>
       </c>
@@ -5493,7 +5494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="117" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A117" t="s">
         <v>18</v>
       </c>
@@ -5531,7 +5532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="118" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A118" t="s">
         <v>18</v>
       </c>
@@ -5569,7 +5570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="119" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A119" t="s">
         <v>18</v>
       </c>
@@ -5607,7 +5608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="120" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A120" t="s">
         <v>18</v>
       </c>
@@ -5645,7 +5646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="121" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A121" t="s">
         <v>18</v>
       </c>
@@ -5683,7 +5684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="122" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A122" t="s">
         <v>18</v>
       </c>
@@ -5721,7 +5722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="123" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A123" t="s">
         <v>18</v>
       </c>
@@ -5759,7 +5760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="124" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A124" t="s">
         <v>19</v>
       </c>
@@ -5797,7 +5798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="125" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A125" t="s">
         <v>19</v>
       </c>
@@ -5835,7 +5836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="126" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A126" t="s">
         <v>19</v>
       </c>
@@ -5873,7 +5874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="127" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A127" t="s">
         <v>19</v>
       </c>
@@ -5911,7 +5912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="128" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A128" t="s">
         <v>19</v>
       </c>
@@ -5949,7 +5950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="129" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A129" t="s">
         <v>19</v>
       </c>
@@ -5987,7 +5988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="130" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A130" t="s">
         <v>19</v>
       </c>
@@ -6025,7 +6026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="131" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A131" t="s">
         <v>19</v>
       </c>
@@ -6063,7 +6064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="132" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A132" t="s">
         <v>19</v>
       </c>
@@ -6101,7 +6102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="133" spans="1:12" hidden="1" x14ac:dyDescent="0.75">
       <c r="A133" t="s">
         <v>19</v>
       </c>
@@ -6140,7 +6141,15 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L133" xr:uid="{EFE1FF5D-95CC-49D0-8C54-8D9CF98199B7}"/>
+  <autoFilter ref="A1:L133" xr:uid="{EFE1FF5D-95CC-49D0-8C54-8D9CF98199B7}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="edu_attending_level123_and_level1_age_d"/>
+        <filter val="edu_attending_level23_and_level2_age_d"/>
+        <filter val="edu_attending_level3_and_level3_age_d"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
making hti demo run
</commit_message>
<xml_diff>
--- a/input_tool/edu_analysistools_loa_AFG.xlsx
+++ b/input_tool/edu_analysistools_loa_AFG.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yann SAY\Desktop\git\EduAnalysisTool\input_tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E01C707C-CF14-4F3B-AE72-B5893F47470F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B48F16D-08DD-4550-AD4D-9A6CA42D7F30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{172E695D-8722-4AF3-920F-94814F3A8B09}"/>
   </bookViews>
@@ -1071,11 +1071,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFE1FF5D-95CC-49D0-8C54-8D9CF98199B7}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:L133"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="H76" sqref="H76"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1124,7 +1123,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1162,7 +1161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1200,7 +1199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -1238,7 +1237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -1276,7 +1275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1314,7 +1313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -1352,7 +1351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -1390,7 +1389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -1428,7 +1427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1466,7 +1465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -1504,7 +1503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1542,7 +1541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -1580,7 +1579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -1618,7 +1617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -1656,7 +1655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -1694,7 +1693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -1732,7 +1731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -1770,7 +1769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -1808,7 +1807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -1846,7 +1845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -1884,7 +1883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -1922,7 +1921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -1960,7 +1959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -1998,7 +1997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -2036,7 +2035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>7</v>
       </c>
@@ -2074,7 +2073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>20</v>
       </c>
@@ -2112,7 +2111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>22</v>
       </c>
@@ -2150,7 +2149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>24</v>
       </c>
@@ -2188,7 +2187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>7</v>
       </c>
@@ -2226,7 +2225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>20</v>
       </c>
@@ -2264,7 +2263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>22</v>
       </c>
@@ -2302,7 +2301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>24</v>
       </c>
@@ -2340,7 +2339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>7</v>
       </c>
@@ -2378,7 +2377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>20</v>
       </c>
@@ -2416,7 +2415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -2454,7 +2453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>24</v>
       </c>
@@ -2492,7 +2491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>7</v>
       </c>
@@ -2530,7 +2529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>20</v>
       </c>
@@ -2568,7 +2567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>22</v>
       </c>
@@ -2606,7 +2605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>24</v>
       </c>
@@ -2644,7 +2643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>30</v>
       </c>
@@ -2682,7 +2681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>26</v>
       </c>
@@ -2720,7 +2719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>30</v>
       </c>
@@ -2758,7 +2757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>26</v>
       </c>
@@ -2796,7 +2795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>30</v>
       </c>
@@ -2834,7 +2833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>26</v>
       </c>
@@ -2872,7 +2871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>30</v>
       </c>
@@ -2910,7 +2909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>26</v>
       </c>
@@ -2948,7 +2947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>30</v>
       </c>
@@ -2986,7 +2985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>26</v>
       </c>
@@ -3024,7 +3023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>30</v>
       </c>
@@ -3062,7 +3061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>26</v>
       </c>
@@ -3100,7 +3099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>26</v>
       </c>
@@ -3138,7 +3137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>30</v>
       </c>
@@ -3176,7 +3175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>26</v>
       </c>
@@ -3214,7 +3213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>30</v>
       </c>
@@ -3252,7 +3251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>30</v>
       </c>
@@ -3290,7 +3289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>26</v>
       </c>
@@ -3328,7 +3327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>30</v>
       </c>
@@ -3366,7 +3365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>26</v>
       </c>
@@ -3404,7 +3403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>10</v>
       </c>
@@ -3442,7 +3441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>10</v>
       </c>
@@ -3480,7 +3479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>10</v>
       </c>
@@ -3518,7 +3517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>10</v>
       </c>
@@ -3556,7 +3555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>10</v>
       </c>
@@ -3594,7 +3593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>10</v>
       </c>
@@ -3632,7 +3631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>10</v>
       </c>
@@ -3670,7 +3669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:12" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:12" ht="15" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>11</v>
       </c>
@@ -3708,7 +3707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:12" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:12" ht="15" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>11</v>
       </c>
@@ -3746,7 +3745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:12" s="2" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:12" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>11</v>
       </c>
@@ -3784,7 +3783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:12" s="2" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:12" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>11</v>
       </c>
@@ -3822,7 +3821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:12" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:12" ht="15" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>11</v>
       </c>
@@ -3860,7 +3859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:12" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:12" ht="15" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>11</v>
       </c>
@@ -3898,7 +3897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:12" ht="15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:12" ht="15" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>11</v>
       </c>
@@ -4734,7 +4733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>35</v>
       </c>
@@ -4772,7 +4771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>35</v>
       </c>
@@ -4810,7 +4809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>35</v>
       </c>
@@ -4848,7 +4847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>35</v>
       </c>
@@ -4886,7 +4885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>35</v>
       </c>
@@ -4924,7 +4923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>35</v>
       </c>
@@ -4962,7 +4961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>36</v>
       </c>
@@ -5000,7 +4999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>36</v>
       </c>
@@ -5038,7 +5037,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>36</v>
       </c>
@@ -5076,7 +5075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>36</v>
       </c>
@@ -5114,7 +5113,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>36</v>
       </c>
@@ -5152,7 +5151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>36</v>
       </c>
@@ -5190,7 +5189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
         <v>7</v>
       </c>
@@ -5228,7 +5227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
         <v>7</v>
       </c>
@@ -5266,7 +5265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>7</v>
       </c>
@@ -5304,7 +5303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>7</v>
       </c>
@@ -5342,7 +5341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>7</v>
       </c>
@@ -5380,7 +5379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>18</v>
       </c>
@@ -5418,7 +5417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>18</v>
       </c>
@@ -5456,7 +5455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>18</v>
       </c>
@@ -5494,7 +5493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>18</v>
       </c>
@@ -5532,7 +5531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>18</v>
       </c>
@@ -5570,7 +5569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>18</v>
       </c>
@@ -5608,7 +5607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>18</v>
       </c>
@@ -5646,7 +5645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>18</v>
       </c>
@@ -5684,7 +5683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>18</v>
       </c>
@@ -5722,7 +5721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>18</v>
       </c>
@@ -5760,7 +5759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>19</v>
       </c>
@@ -5798,7 +5797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>19</v>
       </c>
@@ -5836,7 +5835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>19</v>
       </c>
@@ -5874,7 +5873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>19</v>
       </c>
@@ -5912,7 +5911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>19</v>
       </c>
@@ -5950,7 +5949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>19</v>
       </c>
@@ -5988,7 +5987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>19</v>
       </c>
@@ -6026,7 +6025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>19</v>
       </c>
@@ -6064,7 +6063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>19</v>
       </c>
@@ -6102,7 +6101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>19</v>
       </c>
@@ -6141,15 +6140,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L133" xr:uid="{EFE1FF5D-95CC-49D0-8C54-8D9CF98199B7}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="edu_attending_level123_and_level1_age_d"/>
-        <filter val="edu_attending_level23_and_level2_age_d"/>
-        <filter val="edu_attending_level3_and_level3_age_d"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:L133" xr:uid="{EFE1FF5D-95CC-49D0-8C54-8D9CF98199B7}"/>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>